<commit_message>
Minor fix in name.
</commit_message>
<xml_diff>
--- a/database/Empleados.xlsx
+++ b/database/Empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\InnovationLab2019\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1944A5B7-B958-405E-A578-499D64CA513C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F26E517-2AA5-45D3-9BD2-50432BEA1969}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{77406EC5-31F3-4B7A-B386-A344DA39DCC7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="335">
   <si>
     <t>Pedro Minetti</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Jimena Irigaray</t>
   </si>
   <si>
-    <t>Fernado Olmos</t>
-  </si>
-  <si>
     <t>Juan Estrada</t>
   </si>
   <si>
@@ -591,9 +588,6 @@
     <t>Nicolás</t>
   </si>
   <si>
-    <t>Fernado</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
@@ -1042,6 +1036,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Fernando Olmos</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1457,7 @@
   <dimension ref="A1:Z91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,13 +1493,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -1512,10 +1509,10 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
@@ -1525,18 +1522,18 @@
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="4">
@@ -1571,14 +1568,14 @@
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="S2" s="4"/>
       <c r="T2" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="4" t="str">
@@ -1588,7 +1585,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4" t="str">
         <f ca="1">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q2, "', '", R2, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L2, " , ", IF(C2="", "NULL", CONCATENATE("'", B2,"/", C2, "'")),", ", K2, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B2,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 74754, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 26668, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4" t="str">
@@ -1598,13 +1595,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="4">
@@ -1639,14 +1636,14 @@
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S3" s="4"/>
       <c r="T3" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="4" t="str">
@@ -1656,7 +1653,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4" t="str">
         <f t="shared" ref="X3:X66" ca="1" si="13">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q3, "', '", R3, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L3, " , ", IF(C3="", "NULL", CONCATENATE("'", B3,"/", C3, "'")),", ", K3, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B3,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 85217, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 28138, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4" t="str">
@@ -1669,10 +1666,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="4">
@@ -1707,14 +1704,14 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S4" s="4"/>
       <c r="T4" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U4" s="4"/>
       <c r="V4" s="4" t="str">
@@ -1724,7 +1721,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 53034, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 32024, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4" t="str">
@@ -1734,13 +1731,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="4">
@@ -1775,10 +1772,10 @@
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S5" s="4"/>
       <c r="T5" s="3"/>
@@ -1790,7 +1787,7 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 88182, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 55446, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4" t="str">
@@ -1800,13 +1797,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="4">
@@ -1841,14 +1838,14 @@
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S6" s="4"/>
       <c r="T6" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U6" s="4"/>
       <c r="V6" s="4" t="str">
@@ -1858,7 +1855,7 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 75600, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 44409, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4" t="str">
@@ -1868,13 +1865,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="4">
@@ -1909,14 +1906,14 @@
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S7" s="4"/>
       <c r="T7" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U7" s="4"/>
       <c r="V7" s="4" t="str">
@@ -1926,7 +1923,7 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 86203, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 11238, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4" t="str">
@@ -1936,13 +1933,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="4">
@@ -1977,14 +1974,14 @@
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S8" s="4"/>
       <c r="T8" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U8" s="4"/>
       <c r="V8" s="4" t="str">
@@ -1994,7 +1991,7 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 15204, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 45415, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4" t="str">
@@ -2004,13 +2001,13 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="4">
@@ -2045,14 +2042,14 @@
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S9" s="4"/>
       <c r="T9" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4" t="str">
@@ -2062,7 +2059,7 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 90306, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 10587, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4" t="str">
@@ -2072,13 +2069,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="4">
@@ -2113,14 +2110,14 @@
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S10" s="4"/>
       <c r="T10" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4" t="str">
@@ -2130,7 +2127,7 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 65731, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 85095, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4" t="str">
@@ -2140,13 +2137,13 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="4">
@@ -2181,14 +2178,14 @@
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S11" s="4"/>
       <c r="T11" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U11" s="4"/>
       <c r="V11" s="4" t="str">
@@ -2198,7 +2195,7 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 93359, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 87697, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4" t="str">
@@ -2208,13 +2205,13 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="4">
@@ -2249,14 +2246,14 @@
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U12" s="4"/>
       <c r="V12" s="4" t="str">
@@ -2266,7 +2263,7 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 61053, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 81948, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4" t="str">
@@ -2279,10 +2276,10 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="4">
@@ -2317,14 +2314,14 @@
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S13" s="4"/>
       <c r="T13" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U13" s="4"/>
       <c r="V13" s="4" t="str">
@@ -2334,7 +2331,7 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 21548, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 80702, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="str">
@@ -2344,13 +2341,13 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="4">
@@ -2385,14 +2382,14 @@
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S14" s="4"/>
       <c r="T14" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4" t="str">
@@ -2402,7 +2399,7 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 63792, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 22047, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4" t="str">
@@ -2412,13 +2409,13 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4">
@@ -2453,14 +2450,14 @@
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S15" s="4"/>
       <c r="T15" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U15" s="4"/>
       <c r="V15" s="4" t="str">
@@ -2470,7 +2467,7 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 99781, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 14671, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4" t="str">
@@ -2480,13 +2477,13 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="4">
@@ -2521,14 +2518,14 @@
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S16" s="4"/>
       <c r="T16" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U16" s="4"/>
       <c r="V16" s="4" t="str">
@@ -2538,7 +2535,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 30382, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 22483, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4" t="str">
@@ -2548,13 +2545,13 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="4">
@@ -2589,14 +2586,14 @@
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S17" s="4"/>
       <c r="T17" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U17" s="4"/>
       <c r="V17" s="4" t="str">
@@ -2606,7 +2603,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 29333, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 71949, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4" t="str">
@@ -2619,10 +2616,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="4">
@@ -2657,14 +2654,14 @@
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S18" s="4"/>
       <c r="T18" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U18" s="4"/>
       <c r="V18" s="4" t="str">
@@ -2674,7 +2671,7 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 38813, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 97294, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4" t="str">
@@ -2684,13 +2681,13 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="4">
@@ -2725,14 +2722,14 @@
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S19" s="4"/>
       <c r="T19" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U19" s="4"/>
       <c r="V19" s="4" t="str">
@@ -2742,7 +2739,7 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 46084, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 85358, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4" t="str">
@@ -2752,13 +2749,13 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="4">
@@ -2793,14 +2790,14 @@
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S20" s="4"/>
       <c r="T20" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4" t="str">
@@ -2810,7 +2807,7 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 40741, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 13414, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4" t="str">
@@ -2820,13 +2817,13 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="4">
@@ -2861,14 +2858,14 @@
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="S21" s="4"/>
       <c r="T21" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U21" s="4"/>
       <c r="V21" s="4" t="str">
@@ -2878,7 +2875,7 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 17434, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 58227, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4" t="str">
@@ -2888,13 +2885,13 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="4">
@@ -2929,14 +2926,14 @@
       </c>
       <c r="P22" s="4"/>
       <c r="Q22" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S22" s="4"/>
       <c r="T22" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4" t="str">
@@ -2946,7 +2943,7 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 84749, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 34880, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4" t="str">
@@ -2959,10 +2956,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="4">
@@ -2997,14 +2994,14 @@
       </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S23" s="4"/>
       <c r="T23" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U23" s="4"/>
       <c r="V23" s="4" t="str">
@@ -3014,7 +3011,7 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 56382, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 92063, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4" t="str">
@@ -3024,13 +3021,13 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="4">
@@ -3065,14 +3062,14 @@
       </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S24" s="4"/>
       <c r="T24" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U24" s="4"/>
       <c r="V24" s="4" t="str">
@@ -3082,7 +3079,7 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 3261, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 38695, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4" t="str">
@@ -3092,13 +3089,13 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="4">
@@ -3133,14 +3130,14 @@
       </c>
       <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="S25" s="4"/>
       <c r="T25" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U25" s="4"/>
       <c r="V25" s="4" t="str">
@@ -3150,7 +3147,7 @@
       <c r="W25" s="4"/>
       <c r="X25" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 32694, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 1883, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4" t="str">
@@ -3160,13 +3157,13 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="4">
@@ -3201,14 +3198,14 @@
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S26" s="4"/>
       <c r="T26" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U26" s="4"/>
       <c r="V26" s="4" t="str">
@@ -3218,7 +3215,7 @@
       <c r="W26" s="4"/>
       <c r="X26" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 51357, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 27014, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="str">
@@ -3231,10 +3228,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="4">
@@ -3269,14 +3266,14 @@
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S27" s="4"/>
       <c r="T27" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U27" s="4"/>
       <c r="V27" s="4" t="str">
@@ -3286,7 +3283,7 @@
       <c r="W27" s="4"/>
       <c r="X27" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 613, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 15832, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4" t="str">
@@ -3296,22 +3293,22 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>13</v>
+        <v>334</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="4">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F28" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>Fernado</v>
+        <v>Fernando</v>
       </c>
       <c r="G28" s="4" t="str">
         <f t="shared" si="16"/>
@@ -3337,14 +3334,14 @@
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="S28" s="4"/>
       <c r="T28" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U28" s="4"/>
       <c r="V28" s="4" t="str">
@@ -3354,23 +3351,23 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernado', 'Olmos', NULL, NULL, 9841, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Olmos', NULL, NULL, 82626, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4" t="str">
         <f t="shared" si="14"/>
-        <v>INSERT INTO [dbo].[CandidateCandidateRole] ([CandidateId], [CandidateRoleId], [StartDate], [EndDate]) SELECT [P].[Id], [PR].[Id], '2015-01-01', NULL FROM [dbo].[Candidate] AS P, [dbo].[CandidateRole] AS [PR] WHERE [P].[FirstName] = 'Fernado' AND [P].[LastName] = 'Olmos' AND [PR].[Code] = 'DEV'</v>
+        <v>INSERT INTO [dbo].[CandidateCandidateRole] ([CandidateId], [CandidateRoleId], [StartDate], [EndDate]) SELECT [P].[Id], [PR].[Id], '2015-01-01', NULL FROM [dbo].[Candidate] AS P, [dbo].[CandidateRole] AS [PR] WHERE [P].[FirstName] = 'Fernando' AND [P].[LastName] = 'Olmos' AND [PR].[Code] = 'DEV'</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="4">
@@ -3405,14 +3402,14 @@
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S29" s="4"/>
       <c r="T29" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U29" s="4"/>
       <c r="V29" s="4" t="str">
@@ -3422,7 +3419,7 @@
       <c r="W29" s="4"/>
       <c r="X29" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 66754, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 1109, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4" t="str">
@@ -3432,13 +3429,13 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="4">
@@ -3473,14 +3470,14 @@
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S30" s="4"/>
       <c r="T30" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U30" s="4"/>
       <c r="V30" s="4" t="str">
@@ -3490,7 +3487,7 @@
       <c r="W30" s="4"/>
       <c r="X30" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 16847, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 8597, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4" t="str">
@@ -3500,13 +3497,13 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="4">
@@ -3541,14 +3538,14 @@
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S31" s="4"/>
       <c r="T31" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U31" s="4"/>
       <c r="V31" s="4" t="str">
@@ -3558,7 +3555,7 @@
       <c r="W31" s="4"/>
       <c r="X31" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 623, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 87776, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4" t="str">
@@ -3568,13 +3565,13 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="4">
@@ -3609,14 +3606,14 @@
       </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S32" s="4"/>
       <c r="T32" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U32" s="4"/>
       <c r="V32" s="4" t="str">
@@ -3626,7 +3623,7 @@
       <c r="W32" s="4"/>
       <c r="X32" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 43996, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 99017, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y32" s="4"/>
       <c r="Z32" s="4" t="str">
@@ -3639,10 +3636,10 @@
         <v>5</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="4">
@@ -3677,14 +3674,14 @@
       </c>
       <c r="P33" s="4"/>
       <c r="Q33" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S33" s="4"/>
       <c r="T33" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U33" s="4"/>
       <c r="V33" s="4" t="str">
@@ -3694,7 +3691,7 @@
       <c r="W33" s="4"/>
       <c r="X33" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 72142, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 28441, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4" t="str">
@@ -3704,13 +3701,13 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="4">
@@ -3745,14 +3742,14 @@
       </c>
       <c r="P34" s="4"/>
       <c r="Q34" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S34" s="4"/>
       <c r="T34" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U34" s="4"/>
       <c r="V34" s="4" t="str">
@@ -3762,7 +3759,7 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 63833, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 11770, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4" t="str">
@@ -3775,10 +3772,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="4">
@@ -3813,14 +3810,14 @@
       </c>
       <c r="P35" s="4"/>
       <c r="Q35" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S35" s="4"/>
       <c r="T35" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U35" s="4"/>
       <c r="V35" s="4" t="str">
@@ -3830,7 +3827,7 @@
       <c r="W35" s="4"/>
       <c r="X35" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 62383, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 27232, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4" t="str">
@@ -3840,13 +3837,13 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="4">
@@ -3881,14 +3878,14 @@
       </c>
       <c r="P36" s="4"/>
       <c r="Q36" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="S36" s="4"/>
       <c r="T36" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U36" s="4"/>
       <c r="V36" s="4" t="str">
@@ -3898,7 +3895,7 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 12136, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 38002, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4" t="str">
@@ -3908,13 +3905,13 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="4">
@@ -3949,14 +3946,14 @@
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R37" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S37" s="4"/>
       <c r="T37" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U37" s="4"/>
       <c r="V37" s="4" t="str">
@@ -3966,7 +3963,7 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 61083, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 77434, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y37" s="4"/>
       <c r="Z37" s="4" t="str">
@@ -3976,13 +3973,13 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="4">
@@ -4017,14 +4014,14 @@
       </c>
       <c r="P38" s="4"/>
       <c r="Q38" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="S38" s="4"/>
       <c r="T38" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U38" s="4"/>
       <c r="V38" s="4" t="str">
@@ -4034,7 +4031,7 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 42696, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 41978, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y38" s="4"/>
       <c r="Z38" s="4" t="str">
@@ -4044,13 +4041,13 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="4">
@@ -4085,14 +4082,14 @@
       </c>
       <c r="P39" s="4"/>
       <c r="Q39" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S39" s="4"/>
       <c r="T39" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U39" s="4"/>
       <c r="V39" s="4" t="str">
@@ -4102,7 +4099,7 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 24551, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 68117, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4" t="str">
@@ -4112,13 +4109,13 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="4">
@@ -4153,14 +4150,14 @@
       </c>
       <c r="P40" s="4"/>
       <c r="Q40" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="S40" s="4"/>
       <c r="T40" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U40" s="4"/>
       <c r="V40" s="4" t="str">
@@ -4170,7 +4167,7 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 5574, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 99790, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4" t="str">
@@ -4180,13 +4177,13 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="4">
@@ -4221,14 +4218,14 @@
       </c>
       <c r="P41" s="4"/>
       <c r="Q41" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S41" s="4"/>
       <c r="T41" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U41" s="4"/>
       <c r="V41" s="4" t="str">
@@ -4238,7 +4235,7 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 97137, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 10946, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4" t="str">
@@ -4251,10 +4248,10 @@
         <v>12</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="4">
@@ -4289,14 +4286,14 @@
       </c>
       <c r="P42" s="4"/>
       <c r="Q42" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S42" s="4"/>
       <c r="T42" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U42" s="4"/>
       <c r="V42" s="4" t="str">
@@ -4306,7 +4303,7 @@
       <c r="W42" s="4"/>
       <c r="X42" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 38472, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 73710, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y42" s="4"/>
       <c r="Z42" s="4" t="str">
@@ -4316,10 +4313,10 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
@@ -4355,14 +4352,14 @@
       </c>
       <c r="P43" s="4"/>
       <c r="Q43" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="S43" s="4"/>
       <c r="T43" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U43" s="4"/>
       <c r="V43" s="4" t="str">
@@ -4372,7 +4369,7 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 42136, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 56929, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4" t="str">
@@ -4382,13 +4379,13 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="4">
@@ -4423,14 +4420,14 @@
       </c>
       <c r="P44" s="4"/>
       <c r="Q44" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S44" s="4"/>
       <c r="T44" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U44" s="4"/>
       <c r="V44" s="4" t="str">
@@ -4440,7 +4437,7 @@
       <c r="W44" s="4"/>
       <c r="X44" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 97324, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 41621, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4" t="str">
@@ -4450,13 +4447,13 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="4">
@@ -4491,14 +4488,14 @@
       </c>
       <c r="P45" s="4"/>
       <c r="Q45" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S45" s="4"/>
       <c r="T45" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U45" s="4"/>
       <c r="V45" s="4" t="str">
@@ -4508,7 +4505,7 @@
       <c r="W45" s="4"/>
       <c r="X45" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 4720, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 65590, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y45" s="4"/>
       <c r="Z45" s="4" t="str">
@@ -4518,10 +4515,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
@@ -4540,7 +4537,7 @@
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K46" s="3">
         <v>1</v>
@@ -4559,14 +4556,14 @@
       </c>
       <c r="P46" s="4"/>
       <c r="Q46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R46" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="R46" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="S46" s="4"/>
       <c r="T46" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4" t="str">
@@ -4576,7 +4573,7 @@
       <c r="W46" s="4"/>
       <c r="X46" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 93210, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 88721, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y46" s="4"/>
       <c r="Z46" s="4" t="str">
@@ -4586,13 +4583,13 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="4">
@@ -4608,10 +4605,10 @@
         <v>Mendizabal</v>
       </c>
       <c r="H47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="3">
@@ -4631,14 +4628,14 @@
       </c>
       <c r="P47" s="4"/>
       <c r="Q47" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S47" s="4"/>
       <c r="T47" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U47" s="4"/>
       <c r="V47" s="4" t="str">
@@ -4648,7 +4645,7 @@
       <c r="W47" s="4"/>
       <c r="X47" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 43294, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 87140, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y47" s="4"/>
       <c r="Z47" s="4" t="str">
@@ -4661,10 +4658,10 @@
         <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="4">
@@ -4699,14 +4696,14 @@
       </c>
       <c r="P48" s="4"/>
       <c r="Q48" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S48" s="4"/>
       <c r="T48" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U48" s="4"/>
       <c r="V48" s="4" t="str">
@@ -4716,7 +4713,7 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 60191, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 51798, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y48" s="4"/>
       <c r="Z48" s="4" t="str">
@@ -4726,13 +4723,13 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="4">
@@ -4767,14 +4764,14 @@
       </c>
       <c r="P49" s="4"/>
       <c r="Q49" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S49" s="4"/>
       <c r="T49" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U49" s="4"/>
       <c r="V49" s="4" t="str">
@@ -4784,7 +4781,7 @@
       <c r="W49" s="4"/>
       <c r="X49" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 51731, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 22781, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y49" s="4"/>
       <c r="Z49" s="4" t="str">
@@ -4794,13 +4791,13 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="4">
@@ -4835,14 +4832,14 @@
       </c>
       <c r="P50" s="4"/>
       <c r="Q50" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R50" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="S50" s="4"/>
       <c r="T50" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U50" s="4"/>
       <c r="V50" s="4" t="str">
@@ -4852,7 +4849,7 @@
       <c r="W50" s="4"/>
       <c r="X50" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 72152, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 44778, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y50" s="4"/>
       <c r="Z50" s="4" t="str">
@@ -4862,13 +4859,13 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="4">
@@ -4903,14 +4900,14 @@
       </c>
       <c r="P51" s="4"/>
       <c r="Q51" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="S51" s="4"/>
       <c r="T51" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U51" s="4"/>
       <c r="V51" s="4" t="str">
@@ -4920,7 +4917,7 @@
       <c r="W51" s="4"/>
       <c r="X51" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 60819, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 694, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y51" s="4"/>
       <c r="Z51" s="4" t="str">
@@ -4930,13 +4927,13 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="4">
@@ -4954,7 +4951,7 @@
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K52" s="3">
         <v>1</v>
@@ -4973,14 +4970,14 @@
       </c>
       <c r="P52" s="4"/>
       <c r="Q52" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S52" s="4"/>
       <c r="T52" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U52" s="4"/>
       <c r="V52" s="4" t="str">
@@ -4990,7 +4987,7 @@
       <c r="W52" s="4"/>
       <c r="X52" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 46378, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 44553, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4" t="str">
@@ -5000,13 +4997,13 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="4">
@@ -5022,13 +5019,13 @@
         <v>Noel Mosqueira</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K53" s="3">
         <v>1</v>
@@ -5047,14 +5044,14 @@
       </c>
       <c r="P53" s="4"/>
       <c r="Q53" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="R53" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="R53" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="S53" s="4"/>
       <c r="T53" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U53" s="4"/>
       <c r="V53" s="4" t="str">
@@ -5064,7 +5061,7 @@
       <c r="W53" s="4"/>
       <c r="X53" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 72229, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 22325, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y53" s="4"/>
       <c r="Z53" s="4" t="str">
@@ -5074,13 +5071,13 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="4">
@@ -5096,10 +5093,10 @@
         <v>González</v>
       </c>
       <c r="H54" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I54" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="I54" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="3">
@@ -5119,14 +5116,14 @@
       </c>
       <c r="P54" s="4"/>
       <c r="Q54" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R54" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S54" s="4"/>
       <c r="T54" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U54" s="4"/>
       <c r="V54" s="4" t="str">
@@ -5136,7 +5133,7 @@
       <c r="W54" s="4"/>
       <c r="X54" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 23624, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 48840, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y54" s="4"/>
       <c r="Z54" s="4" t="str">
@@ -5146,13 +5143,13 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="4">
@@ -5187,14 +5184,14 @@
       </c>
       <c r="P55" s="4"/>
       <c r="Q55" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="R55" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S55" s="4"/>
       <c r="T55" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U55" s="4"/>
       <c r="V55" s="4" t="str">
@@ -5204,7 +5201,7 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 39969, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 73480, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y55" s="4"/>
       <c r="Z55" s="4" t="str">
@@ -5214,13 +5211,13 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D56" s="8"/>
       <c r="E56" s="4">
@@ -5255,14 +5252,14 @@
       </c>
       <c r="P56" s="4"/>
       <c r="Q56" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="R56" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S56" s="4"/>
       <c r="T56" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U56" s="4"/>
       <c r="V56" s="4" t="str">
@@ -5272,7 +5269,7 @@
       <c r="W56" s="4"/>
       <c r="X56" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 1128, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 49702, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y56" s="4"/>
       <c r="Z56" s="4" t="str">
@@ -5282,13 +5279,13 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="4">
@@ -5323,14 +5320,14 @@
       </c>
       <c r="P57" s="4"/>
       <c r="Q57" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="R57" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S57" s="4"/>
       <c r="T57" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U57" s="4"/>
       <c r="V57" s="4" t="str">
@@ -5340,7 +5337,7 @@
       <c r="W57" s="4"/>
       <c r="X57" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 20254, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 39123, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y57" s="4"/>
       <c r="Z57" s="4" t="str">
@@ -5350,13 +5347,13 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="4">
@@ -5391,14 +5388,14 @@
       </c>
       <c r="P58" s="4"/>
       <c r="Q58" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R58" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S58" s="4"/>
       <c r="T58" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U58" s="4"/>
       <c r="V58" s="4" t="str">
@@ -5408,7 +5405,7 @@
       <c r="W58" s="4"/>
       <c r="X58" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 47101, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 5881, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y58" s="4"/>
       <c r="Z58" s="4" t="str">
@@ -5418,13 +5415,13 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="4">
@@ -5459,14 +5456,14 @@
       </c>
       <c r="P59" s="4"/>
       <c r="Q59" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R59" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S59" s="4"/>
       <c r="T59" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U59" s="4"/>
       <c r="V59" s="4" t="str">
@@ -5476,7 +5473,7 @@
       <c r="W59" s="4"/>
       <c r="X59" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 90817, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 67603, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y59" s="4"/>
       <c r="Z59" s="4" t="str">
@@ -5486,13 +5483,13 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="4">
@@ -5527,14 +5524,14 @@
       </c>
       <c r="P60" s="4"/>
       <c r="Q60" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R60" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S60" s="4"/>
       <c r="T60" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U60" s="4"/>
       <c r="V60" s="4" t="str">
@@ -5544,7 +5541,7 @@
       <c r="W60" s="4"/>
       <c r="X60" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 31459, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 57049, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y60" s="4"/>
       <c r="Z60" s="4" t="str">
@@ -5554,13 +5551,13 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="4">
@@ -5595,10 +5592,10 @@
       </c>
       <c r="P61" s="4"/>
       <c r="Q61" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="R61" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="S61" s="4"/>
       <c r="T61" s="3"/>
@@ -5610,7 +5607,7 @@
       <c r="W61" s="4"/>
       <c r="X61" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 33156, 0 , 'MVD/Nicolas_Ma¤ay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 74755, 0 , 'MVD/Nicolas_Ma¤ay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y61" s="4"/>
       <c r="Z61" s="4" t="str">
@@ -5620,13 +5617,13 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="4">
@@ -5661,14 +5658,14 @@
       </c>
       <c r="P62" s="4"/>
       <c r="Q62" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="R62" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S62" s="4"/>
       <c r="T62" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U62" s="4"/>
       <c r="V62" s="4" t="str">
@@ -5678,7 +5675,7 @@
       <c r="W62" s="4"/>
       <c r="X62" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 66238, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 4576, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y62" s="4"/>
       <c r="Z62" s="4" t="str">
@@ -5688,13 +5685,13 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="4">
@@ -5729,14 +5726,14 @@
       </c>
       <c r="P63" s="4"/>
       <c r="Q63" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R63" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="S63" s="4"/>
       <c r="T63" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U63" s="4"/>
       <c r="V63" s="4" t="str">
@@ -5746,7 +5743,7 @@
       <c r="W63" s="4"/>
       <c r="X63" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 4895, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 40129, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y63" s="4"/>
       <c r="Z63" s="4" t="str">
@@ -5759,10 +5756,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="4">
@@ -5797,14 +5794,14 @@
       </c>
       <c r="P64" s="4"/>
       <c r="Q64" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R64" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S64" s="4"/>
       <c r="T64" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U64" s="4"/>
       <c r="V64" s="4" t="str">
@@ -5814,7 +5811,7 @@
       <c r="W64" s="4"/>
       <c r="X64" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 99782, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 43445, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y64" s="4"/>
       <c r="Z64" s="4" t="str">
@@ -5824,13 +5821,13 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="4">
@@ -5865,14 +5862,14 @@
       </c>
       <c r="P65" s="4"/>
       <c r="Q65" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R65" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S65" s="4"/>
       <c r="T65" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U65" s="4"/>
       <c r="V65" s="4" t="str">
@@ -5882,7 +5879,7 @@
       <c r="W65" s="4"/>
       <c r="X65" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 26861, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 40018, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y65" s="4"/>
       <c r="Z65" s="4" t="str">
@@ -5892,10 +5889,10 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
@@ -5931,14 +5928,14 @@
       </c>
       <c r="P66" s="4"/>
       <c r="Q66" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R66" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="S66" s="4"/>
       <c r="T66" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U66" s="4"/>
       <c r="V66" s="4" t="str">
@@ -5948,7 +5945,7 @@
       <c r="W66" s="4"/>
       <c r="X66" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 27905, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 68469, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y66" s="4"/>
       <c r="Z66" s="4" t="str">
@@ -5958,13 +5955,13 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="4">
@@ -5999,14 +5996,14 @@
       </c>
       <c r="P67" s="4"/>
       <c r="Q67" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R67" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S67" s="4"/>
       <c r="T67" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U67" s="4"/>
       <c r="V67" s="4" t="str">
@@ -6016,7 +6013,7 @@
       <c r="W67" s="4"/>
       <c r="X67" s="4" t="str">
         <f t="shared" ref="X67:X91" ca="1" si="23">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q67, "', '", R67, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L67, " , ", IF(C67="", "NULL", CONCATENATE("'", B67,"/", C67, "'")),", ", K67, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B67,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 17716, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 93693, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y67" s="4"/>
       <c r="Z67" s="4" t="str">
@@ -6026,13 +6023,13 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="4">
@@ -6067,14 +6064,14 @@
       </c>
       <c r="P68" s="4"/>
       <c r="Q68" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R68" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S68" s="4"/>
       <c r="T68" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U68" s="4"/>
       <c r="V68" s="4" t="str">
@@ -6084,7 +6081,7 @@
       <c r="W68" s="4"/>
       <c r="X68" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 68963, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 33430, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y68" s="4"/>
       <c r="Z68" s="4" t="str">
@@ -6097,10 +6094,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="4">
@@ -6135,14 +6132,14 @@
       </c>
       <c r="P69" s="4"/>
       <c r="Q69" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R69" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S69" s="4"/>
       <c r="T69" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U69" s="4"/>
       <c r="V69" s="4" t="str">
@@ -6152,7 +6149,7 @@
       <c r="W69" s="4"/>
       <c r="X69" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 2248, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 48586, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y69" s="4"/>
       <c r="Z69" s="4" t="str">
@@ -6162,13 +6159,13 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="4">
@@ -6203,14 +6200,14 @@
       </c>
       <c r="P70" s="4"/>
       <c r="Q70" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R70" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S70" s="4"/>
       <c r="T70" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U70" s="4"/>
       <c r="V70" s="4" t="str">
@@ -6220,7 +6217,7 @@
       <c r="W70" s="4"/>
       <c r="X70" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 76415, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 73668, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y70" s="4"/>
       <c r="Z70" s="4" t="str">
@@ -6230,13 +6227,13 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="4">
@@ -6271,14 +6268,14 @@
       </c>
       <c r="P71" s="4"/>
       <c r="Q71" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="R71" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S71" s="4"/>
       <c r="T71" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U71" s="4"/>
       <c r="V71" s="4" t="str">
@@ -6288,7 +6285,7 @@
       <c r="W71" s="4"/>
       <c r="X71" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 99794, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 5725, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y71" s="4"/>
       <c r="Z71" s="4" t="str">
@@ -6298,13 +6295,13 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="4">
@@ -6339,14 +6336,14 @@
       </c>
       <c r="P72" s="4"/>
       <c r="Q72" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="R72" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S72" s="4"/>
       <c r="T72" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U72" s="4"/>
       <c r="V72" s="4" t="str">
@@ -6356,7 +6353,7 @@
       <c r="W72" s="4"/>
       <c r="X72" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 36371, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 55432, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y72" s="4"/>
       <c r="Z72" s="4" t="str">
@@ -6366,13 +6363,13 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="4">
@@ -6407,14 +6404,14 @@
       </c>
       <c r="P73" s="4"/>
       <c r="Q73" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R73" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S73" s="4"/>
       <c r="T73" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U73" s="4"/>
       <c r="V73" s="4" t="str">
@@ -6424,7 +6421,7 @@
       <c r="W73" s="4"/>
       <c r="X73" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 41950, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 94231, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y73" s="4"/>
       <c r="Z73" s="4" t="str">
@@ -6434,13 +6431,13 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="4">
@@ -6475,14 +6472,14 @@
       </c>
       <c r="P74" s="4"/>
       <c r="Q74" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R74" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S74" s="4"/>
       <c r="T74" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U74" s="4"/>
       <c r="V74" s="4" t="str">
@@ -6492,7 +6489,7 @@
       <c r="W74" s="4"/>
       <c r="X74" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 92468, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 90191, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y74" s="4"/>
       <c r="Z74" s="4" t="str">
@@ -6505,10 +6502,10 @@
         <v>3</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D75" s="8"/>
       <c r="E75" s="4">
@@ -6543,14 +6540,14 @@
       </c>
       <c r="P75" s="4"/>
       <c r="Q75" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="R75" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S75" s="4"/>
       <c r="T75" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U75" s="4"/>
       <c r="V75" s="4" t="str">
@@ -6560,7 +6557,7 @@
       <c r="W75" s="4"/>
       <c r="X75" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 27064, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 16796, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y75" s="4"/>
       <c r="Z75" s="4" t="str">
@@ -6570,13 +6567,13 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="4">
@@ -6611,14 +6608,14 @@
       </c>
       <c r="P76" s="4"/>
       <c r="Q76" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R76" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S76" s="4"/>
       <c r="T76" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U76" s="4"/>
       <c r="V76" s="4" t="str">
@@ -6628,7 +6625,7 @@
       <c r="W76" s="4"/>
       <c r="X76" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 24237, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 57440, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y76" s="4"/>
       <c r="Z76" s="4" t="str">
@@ -6641,10 +6638,10 @@
         <v>4</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="4">
@@ -6679,14 +6676,14 @@
       </c>
       <c r="P77" s="4"/>
       <c r="Q77" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R77" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S77" s="4"/>
       <c r="T77" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U77" s="4"/>
       <c r="V77" s="4" t="str">
@@ -6696,7 +6693,7 @@
       <c r="W77" s="4"/>
       <c r="X77" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 55528, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 20719, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y77" s="4"/>
       <c r="Z77" s="4" t="str">
@@ -6706,13 +6703,13 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D78" s="8"/>
       <c r="E78" s="4">
@@ -6747,14 +6744,14 @@
       </c>
       <c r="P78" s="4"/>
       <c r="Q78" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="R78" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S78" s="4"/>
       <c r="T78" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U78" s="4"/>
       <c r="V78" s="4" t="str">
@@ -6764,7 +6761,7 @@
       <c r="W78" s="4"/>
       <c r="X78" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 76052, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 89634, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y78" s="4"/>
       <c r="Z78" s="4" t="str">
@@ -6774,13 +6771,13 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="4">
@@ -6815,14 +6812,14 @@
       </c>
       <c r="P79" s="4"/>
       <c r="Q79" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R79" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S79" s="4"/>
       <c r="T79" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="U79" s="4"/>
       <c r="V79" s="4" t="str">
@@ -6832,7 +6829,7 @@
       <c r="W79" s="4"/>
       <c r="X79" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 82032, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 84914, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y79" s="4"/>
       <c r="Z79" s="4" t="str">
@@ -6842,13 +6839,13 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="4">
@@ -6883,14 +6880,14 @@
       </c>
       <c r="P80" s="4"/>
       <c r="Q80" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R80" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S80" s="4"/>
       <c r="T80" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U80" s="4"/>
       <c r="V80" s="4" t="str">
@@ -6900,7 +6897,7 @@
       <c r="W80" s="4"/>
       <c r="X80" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 70846, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 32214, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y80" s="4"/>
       <c r="Z80" s="4" t="str">
@@ -6910,13 +6907,13 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="4">
@@ -6951,14 +6948,14 @@
       </c>
       <c r="P81" s="4"/>
       <c r="Q81" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R81" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S81" s="4"/>
       <c r="T81" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="U81" s="4"/>
       <c r="V81" s="4" t="str">
@@ -6968,7 +6965,7 @@
       <c r="W81" s="4"/>
       <c r="X81" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 46842, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 75257, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y81" s="4"/>
       <c r="Z81" s="4" t="str">
@@ -6978,13 +6975,13 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="4">
@@ -7019,14 +7016,14 @@
       </c>
       <c r="P82" s="4"/>
       <c r="Q82" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R82" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S82" s="4"/>
       <c r="T82" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U82" s="4"/>
       <c r="V82" s="4" t="str">
@@ -7036,7 +7033,7 @@
       <c r="W82" s="4"/>
       <c r="X82" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 96537, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 14042, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y82" s="4"/>
       <c r="Z82" s="4" t="str">
@@ -7046,13 +7043,13 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="4">
@@ -7087,14 +7084,14 @@
       </c>
       <c r="P83" s="4"/>
       <c r="Q83" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R83" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="S83" s="4"/>
       <c r="T83" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U83" s="4"/>
       <c r="V83" s="4" t="str">
@@ -7104,7 +7101,7 @@
       <c r="W83" s="4"/>
       <c r="X83" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 84685, 0 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 74060, 0 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4" t="str">
@@ -7114,13 +7111,13 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="4">
@@ -7155,14 +7152,14 @@
       </c>
       <c r="P84" s="4"/>
       <c r="Q84" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R84" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="S84" s="4"/>
       <c r="T84" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U84" s="4"/>
       <c r="V84" s="4" t="str">
@@ -7172,7 +7169,7 @@
       <c r="W84" s="4"/>
       <c r="X84" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 51726, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 59124, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y84" s="4"/>
       <c r="Z84" s="4" t="str">
@@ -7182,13 +7179,13 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="4">
@@ -7223,14 +7220,14 @@
       </c>
       <c r="P85" s="4"/>
       <c r="Q85" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R85" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S85" s="4"/>
       <c r="T85" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U85" s="4"/>
       <c r="V85" s="4" t="str">
@@ -7240,7 +7237,7 @@
       <c r="W85" s="4"/>
       <c r="X85" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 67741, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 44482, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y85" s="4"/>
       <c r="Z85" s="4" t="str">
@@ -7250,13 +7247,13 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="4">
@@ -7291,14 +7288,14 @@
       </c>
       <c r="P86" s="4"/>
       <c r="Q86" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R86" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S86" s="4"/>
       <c r="T86" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="U86" s="4"/>
       <c r="V86" s="4" t="str">
@@ -7308,7 +7305,7 @@
       <c r="W86" s="4"/>
       <c r="X86" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 67755, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 24173, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y86" s="4"/>
       <c r="Z86" s="4" t="str">
@@ -7318,10 +7315,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
@@ -7361,11 +7358,11 @@
         <v>Adrián</v>
       </c>
       <c r="R87" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S87" s="4"/>
       <c r="T87" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="U87" s="4"/>
       <c r="V87" s="4" t="str">
@@ -7375,7 +7372,7 @@
       <c r="W87" s="4"/>
       <c r="X87" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 54405, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 20716, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y87" s="4"/>
       <c r="Z87" s="4" t="str">
@@ -7385,10 +7382,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="8"/>
@@ -7428,11 +7425,11 @@
         <v>Agustín</v>
       </c>
       <c r="R88" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="S88" s="4"/>
       <c r="T88" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U88" s="4"/>
       <c r="V88" s="4" t="str">
@@ -7442,7 +7439,7 @@
       <c r="W88" s="4"/>
       <c r="X88" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 10264, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 41959, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y88" s="4"/>
       <c r="Z88" s="4" t="str">
@@ -7452,10 +7449,10 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
@@ -7495,11 +7492,11 @@
         <v>Andrea</v>
       </c>
       <c r="R89" s="4" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="S89" s="4"/>
       <c r="T89" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="U89" s="4"/>
       <c r="V89" s="4" t="str">
@@ -7509,7 +7506,7 @@
       <c r="W89" s="4"/>
       <c r="X89" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 36416, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 51786, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y89" s="4"/>
       <c r="Z89" s="4" t="str">
@@ -7519,10 +7516,10 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>324</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="8"/>
@@ -7562,11 +7559,11 @@
         <v>Ezequiel</v>
       </c>
       <c r="R90" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S90" s="4"/>
       <c r="T90" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U90" s="4"/>
       <c r="V90" s="4" t="str">
@@ -7576,7 +7573,7 @@
       <c r="W90" s="4"/>
       <c r="X90" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 16910, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 3250, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y90" s="4"/>
       <c r="Z90" s="4" t="str">
@@ -7586,10 +7583,10 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="8"/>
@@ -7629,11 +7626,11 @@
         <v>Luis</v>
       </c>
       <c r="R91" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="S91" s="4"/>
       <c r="T91" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U91" s="4"/>
       <c r="V91" s="4" t="str">
@@ -7643,7 +7640,7 @@
       <c r="W91" s="4"/>
       <c r="X91" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 60570, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 42218, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y91" s="4"/>
       <c r="Z91" s="4" t="str">
@@ -7671,12 +7668,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0B7B36A0A09E458158046810038137" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bafe724513c9d1f26c4bf7dd6ed8389c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="03dca61d-4bd9-44e4-bb28-2e245975cefa" xmlns:ns4="58628ce2-31db-48c9-83e7-9ec9dce11b86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1eeb2709ac0754591c2d8728cadbcbe3" ns3:_="" ns4:_="">
     <xsd:import namespace="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
@@ -7885,6 +7876,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6844CB-EC2C-4324-A58D-DA98579E50A5}">
   <ds:schemaRefs>
@@ -7894,23 +7891,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2396B7-CB8B-47A8-AF89-5D1D70206F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7927,4 +7907,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Menu redesign and region components added.
</commit_message>
<xml_diff>
--- a/database/Empleados.xlsx
+++ b/database/Empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\InnovationLab2019\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0000E9E7-18C8-4714-9D8B-7B876F9594AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC3C6-A14D-419F-A485-38571747F6D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{77406EC5-31F3-4B7A-B386-A344DA39DCC7}"/>
   </bookViews>
@@ -870,9 +870,6 @@
     <t>Nicolas_Lasarte.JPG</t>
   </si>
   <si>
-    <t>Nicolas_Ma¤ay.jpg</t>
-  </si>
-  <si>
     <t>Pablo_Cawen.JPG</t>
   </si>
   <si>
@@ -1039,6 +1036,9 @@
   </si>
   <si>
     <t>OPS</t>
+  </si>
+  <si>
+    <t>Nicolas_Manay.jpg</t>
   </si>
 </sst>
 </file>
@@ -1456,7 +1456,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F6A38B-9221-46B4-8760-38B60FB5A75C}">
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1491,13 +1494,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -1507,10 +1510,10 @@
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>330</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>331</v>
       </c>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
@@ -1520,18 +1523,18 @@
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>324</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>325</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="4">
@@ -1569,7 +1572,7 @@
         <v>172</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S2" s="4"/>
       <c r="T2" s="3" t="s">
@@ -1583,7 +1586,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4" t="str">
         <f ca="1">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q2, "', '", R2, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L2, " , ", IF(C2="", "NULL", CONCATENATE("'", B2,"/", C2, "'")),", ", K2, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B2,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 47832, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 35784, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4" t="str">
@@ -1596,7 +1599,7 @@
         <v>65</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>231</v>
@@ -1651,7 +1654,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4" t="str">
         <f t="shared" ref="X3:X66" ca="1" si="13">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q3, "', '", R3, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L3, " , ", IF(C3="", "NULL", CONCATENATE("'", B3,"/", C3, "'")),", ", K3, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B3,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 66448, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 6311, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4" t="str">
@@ -1664,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>232</v>
@@ -1719,7 +1722,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 47134, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 43714, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4" t="str">
@@ -1732,7 +1735,7 @@
         <v>76</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>233</v>
@@ -1785,7 +1788,7 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 27828, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 20374, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4" t="str">
@@ -1798,7 +1801,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>234</v>
@@ -1853,7 +1856,7 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 61733, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 84910, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4" t="str">
@@ -1866,10 +1869,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="4">
@@ -1921,7 +1924,7 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 67287, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 26051, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4" t="str">
@@ -1934,7 +1937,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>235</v>
@@ -1989,7 +1992,7 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 17487, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 19037, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4" t="str">
@@ -2002,7 +2005,7 @@
         <v>53</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>236</v>
@@ -2057,7 +2060,7 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 6639, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 52268, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4" t="str">
@@ -2070,7 +2073,7 @@
         <v>78</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>237</v>
@@ -2125,7 +2128,7 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 32954, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 32425, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4" t="str">
@@ -2138,7 +2141,7 @@
         <v>73</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>238</v>
@@ -2193,7 +2196,7 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 72142, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 45664, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4" t="str">
@@ -2206,7 +2209,7 @@
         <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>239</v>
@@ -2261,7 +2264,7 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 84546, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 92386, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4" t="str">
@@ -2274,7 +2277,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>240</v>
@@ -2329,7 +2332,7 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 81521, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 7422, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="str">
@@ -2342,7 +2345,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>241</v>
@@ -2397,7 +2400,7 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 41119, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 99959, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4" t="str">
@@ -2410,10 +2413,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="4">
@@ -2465,7 +2468,7 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 27490, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 15041, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4" t="str">
@@ -2478,7 +2481,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>242</v>
@@ -2533,7 +2536,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 23332, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 43661, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4" t="str">
@@ -2546,7 +2549,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>243</v>
@@ -2601,7 +2604,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 3918, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 90404, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4" t="str">
@@ -2614,7 +2617,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>244</v>
@@ -2669,7 +2672,7 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 7818, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 98529, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4" t="str">
@@ -2682,7 +2685,7 @@
         <v>56</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>245</v>
@@ -2737,7 +2740,7 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 73333, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 88897, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4" t="str">
@@ -2750,7 +2753,7 @@
         <v>70</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>246</v>
@@ -2805,7 +2808,7 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 50780, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 29711, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4" t="str">
@@ -2818,7 +2821,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>247</v>
@@ -2873,7 +2876,7 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 54107, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 68703, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4" t="str">
@@ -2886,7 +2889,7 @@
         <v>44</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>248</v>
@@ -2941,7 +2944,7 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 96320, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 14945, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4" t="str">
@@ -2954,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>249</v>
@@ -3009,7 +3012,7 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 12591, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 77885, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4" t="str">
@@ -3022,7 +3025,7 @@
         <v>45</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>272</v>
@@ -3077,7 +3080,7 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 58787, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 30892, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4" t="str">
@@ -3090,10 +3093,10 @@
         <v>31</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="4">
@@ -3145,7 +3148,7 @@
       <c r="W25" s="4"/>
       <c r="X25" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 29051, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 49652, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4" t="str">
@@ -3158,7 +3161,7 @@
         <v>69</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>250</v>
@@ -3213,7 +3216,7 @@
       <c r="W26" s="4"/>
       <c r="X26" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 28403, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 28970, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="str">
@@ -3226,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>251</v>
@@ -3281,7 +3284,7 @@
       <c r="W27" s="4"/>
       <c r="X27" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 88726, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 14927, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4" t="str">
@@ -3291,13 +3294,13 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="4">
@@ -3349,7 +3352,7 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Olmos', NULL, NULL, 29497, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Olmos', NULL, NULL, 18091, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4" t="str">
@@ -3362,7 +3365,7 @@
         <v>55</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>252</v>
@@ -3417,7 +3420,7 @@
       <c r="W29" s="4"/>
       <c r="X29" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 75489, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 14265, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4" t="str">
@@ -3430,7 +3433,7 @@
         <v>38</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>253</v>
@@ -3485,7 +3488,7 @@
       <c r="W30" s="4"/>
       <c r="X30" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 42808, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 99801, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4" t="str">
@@ -3498,7 +3501,7 @@
         <v>79</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>254</v>
@@ -3553,7 +3556,7 @@
       <c r="W31" s="4"/>
       <c r="X31" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 52557, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 50773, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4" t="str">
@@ -3566,7 +3569,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>255</v>
@@ -3621,7 +3624,7 @@
       <c r="W32" s="4"/>
       <c r="X32" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 48782, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 39303, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y32" s="4"/>
       <c r="Z32" s="4" t="str">
@@ -3634,7 +3637,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>256</v>
@@ -3689,7 +3692,7 @@
       <c r="W33" s="4"/>
       <c r="X33" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 46028, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 91940, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4" t="str">
@@ -3702,7 +3705,7 @@
         <v>72</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>257</v>
@@ -3757,7 +3760,7 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 79045, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 28288, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4" t="str">
@@ -3770,7 +3773,7 @@
         <v>11</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>258</v>
@@ -3825,7 +3828,7 @@
       <c r="W35" s="4"/>
       <c r="X35" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 84536, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 49637, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4" t="str">
@@ -3838,7 +3841,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>259</v>
@@ -3893,7 +3896,7 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 94651, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 7576, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4" t="str">
@@ -3906,7 +3909,7 @@
         <v>30</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>260</v>
@@ -3961,7 +3964,7 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 72193, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 73354, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y37" s="4"/>
       <c r="Z37" s="4" t="str">
@@ -3974,7 +3977,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>261</v>
@@ -4029,7 +4032,7 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 58297, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 5691, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y38" s="4"/>
       <c r="Z38" s="4" t="str">
@@ -4042,10 +4045,10 @@
         <v>54</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="4">
@@ -4097,7 +4100,7 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 96248, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 29540, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4" t="str">
@@ -4110,7 +4113,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>262</v>
@@ -4165,7 +4168,7 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 64412, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 74509, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4" t="str">
@@ -4178,7 +4181,7 @@
         <v>27</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>263</v>
@@ -4233,7 +4236,7 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 29202, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 3486, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4" t="str">
@@ -4246,10 +4249,10 @@
         <v>12</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="4">
@@ -4301,7 +4304,7 @@
       <c r="W42" s="4"/>
       <c r="X42" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 67362, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 39030, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y42" s="4"/>
       <c r="Z42" s="4" t="str">
@@ -4314,7 +4317,7 @@
         <v>61</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="8"/>
@@ -4367,7 +4370,7 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 87660, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 69887, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4" t="str">
@@ -4380,7 +4383,7 @@
         <v>22</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>264</v>
@@ -4435,7 +4438,7 @@
       <c r="W44" s="4"/>
       <c r="X44" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 90351, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 77954, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4" t="str">
@@ -4448,10 +4451,10 @@
         <v>13</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D45" s="8"/>
       <c r="E45" s="4">
@@ -4503,7 +4506,7 @@
       <c r="W45" s="4"/>
       <c r="X45" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 15982, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 37884, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y45" s="4"/>
       <c r="Z45" s="4" t="str">
@@ -4516,7 +4519,7 @@
         <v>62</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
@@ -4561,7 +4564,7 @@
       </c>
       <c r="S46" s="4"/>
       <c r="T46" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4" t="str">
@@ -4571,7 +4574,7 @@
       <c r="W46" s="4"/>
       <c r="X46" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 9750, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 40324, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y46" s="4"/>
       <c r="Z46" s="4" t="str">
@@ -4584,7 +4587,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>265</v>
@@ -4643,7 +4646,7 @@
       <c r="W47" s="4"/>
       <c r="X47" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 60590, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 60134, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y47" s="4"/>
       <c r="Z47" s="4" t="str">
@@ -4656,7 +4659,7 @@
         <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>266</v>
@@ -4711,7 +4714,7 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 51820, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 39612, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y48" s="4"/>
       <c r="Z48" s="4" t="str">
@@ -4724,7 +4727,7 @@
         <v>58</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>267</v>
@@ -4779,7 +4782,7 @@
       <c r="W49" s="4"/>
       <c r="X49" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 85470, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 3929, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y49" s="4"/>
       <c r="Z49" s="4" t="str">
@@ -4792,7 +4795,7 @@
         <v>37</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>268</v>
@@ -4847,7 +4850,7 @@
       <c r="W50" s="4"/>
       <c r="X50" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 23144, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 37694, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y50" s="4"/>
       <c r="Z50" s="4" t="str">
@@ -4860,7 +4863,7 @@
         <v>29</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>269</v>
@@ -4915,7 +4918,7 @@
       <c r="W51" s="4"/>
       <c r="X51" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 63356, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 29742, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y51" s="4"/>
       <c r="Z51" s="4" t="str">
@@ -4928,7 +4931,7 @@
         <v>85</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>270</v>
@@ -4985,7 +4988,7 @@
       <c r="W52" s="4"/>
       <c r="X52" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 96249, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 89047, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4" t="str">
@@ -4998,7 +5001,7 @@
         <v>82</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>271</v>
@@ -5059,7 +5062,7 @@
       <c r="W53" s="4"/>
       <c r="X53" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 74226, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 33754, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y53" s="4"/>
       <c r="Z53" s="4" t="str">
@@ -5072,10 +5075,10 @@
         <v>77</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="4">
@@ -5131,7 +5134,7 @@
       <c r="W54" s="4"/>
       <c r="X54" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 66323, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 84184, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y54" s="4"/>
       <c r="Z54" s="4" t="str">
@@ -5144,7 +5147,7 @@
         <v>64</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>273</v>
@@ -5199,7 +5202,7 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 40698, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 3588, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y55" s="4"/>
       <c r="Z55" s="4" t="str">
@@ -5212,7 +5215,7 @@
         <v>23</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>274</v>
@@ -5267,7 +5270,7 @@
       <c r="W56" s="4"/>
       <c r="X56" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 95134, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 13190, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y56" s="4"/>
       <c r="Z56" s="4" t="str">
@@ -5280,7 +5283,7 @@
         <v>88</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>275</v>
@@ -5335,7 +5338,7 @@
       <c r="W57" s="4"/>
       <c r="X57" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 81212, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 14542, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y57" s="4"/>
       <c r="Z57" s="4" t="str">
@@ -5348,10 +5351,10 @@
         <v>34</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="4">
@@ -5403,7 +5406,7 @@
       <c r="W58" s="4"/>
       <c r="X58" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 19250, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 59697, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y58" s="4"/>
       <c r="Z58" s="4" t="str">
@@ -5416,7 +5419,7 @@
         <v>68</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>276</v>
@@ -5471,7 +5474,7 @@
       <c r="W59" s="4"/>
       <c r="X59" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 88577, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 40774, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y59" s="4"/>
       <c r="Z59" s="4" t="str">
@@ -5484,7 +5487,7 @@
         <v>67</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>277</v>
@@ -5539,7 +5542,7 @@
       <c r="W60" s="4"/>
       <c r="X60" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 66884, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 5630, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y60" s="4"/>
       <c r="Z60" s="4" t="str">
@@ -5552,10 +5555,10 @@
         <v>42</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>278</v>
+        <v>334</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="4">
@@ -5582,7 +5585,7 @@
       <c r="M61" s="4"/>
       <c r="N61" s="4" t="str">
         <f t="shared" si="17"/>
-        <v>Nicolas_Ma¤ay.jpg</v>
+        <v>Nicolas_Manay.jpg</v>
       </c>
       <c r="O61" s="4" t="str">
         <f t="shared" si="18"/>
@@ -5605,7 +5608,7 @@
       <c r="W61" s="4"/>
       <c r="X61" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 57499, 0 , 'MVD/Nicolas_Ma¤ay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 53862, 0 , 'MVD/Nicolas_Manay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y61" s="4"/>
       <c r="Z61" s="4" t="str">
@@ -5618,10 +5621,10 @@
         <v>41</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="4">
@@ -5673,7 +5676,7 @@
       <c r="W62" s="4"/>
       <c r="X62" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 16656, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 84708, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y62" s="4"/>
       <c r="Z62" s="4" t="str">
@@ -5686,10 +5689,10 @@
         <v>35</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="4">
@@ -5741,7 +5744,7 @@
       <c r="W63" s="4"/>
       <c r="X63" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 53695, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 58230, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y63" s="4"/>
       <c r="Z63" s="4" t="str">
@@ -5754,10 +5757,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="4">
@@ -5809,7 +5812,7 @@
       <c r="W64" s="4"/>
       <c r="X64" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 39886, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 97695, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y64" s="4"/>
       <c r="Z64" s="4" t="str">
@@ -5822,10 +5825,10 @@
         <v>71</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="4">
@@ -5877,7 +5880,7 @@
       <c r="W65" s="4"/>
       <c r="X65" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 5302, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 32040, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y65" s="4"/>
       <c r="Z65" s="4" t="str">
@@ -5890,7 +5893,7 @@
         <v>60</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
@@ -5933,7 +5936,7 @@
       </c>
       <c r="S66" s="4"/>
       <c r="T66" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U66" s="4"/>
       <c r="V66" s="4" t="str">
@@ -5943,7 +5946,7 @@
       <c r="W66" s="4"/>
       <c r="X66" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 12378, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 29456, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y66" s="4"/>
       <c r="Z66" s="4" t="str">
@@ -5956,10 +5959,10 @@
         <v>20</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="4">
@@ -6011,7 +6014,7 @@
       <c r="W67" s="4"/>
       <c r="X67" s="4" t="str">
         <f t="shared" ref="X67:X91" ca="1" si="23">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q67, "', '", R67, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L67, " , ", IF(C67="", "NULL", CONCATENATE("'", B67,"/", C67, "'")),", ", K67, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B67,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 54293, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 46159, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y67" s="4"/>
       <c r="Z67" s="4" t="str">
@@ -6024,10 +6027,10 @@
         <v>52</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="4">
@@ -6079,7 +6082,7 @@
       <c r="W68" s="4"/>
       <c r="X68" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 48674, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 97358, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y68" s="4"/>
       <c r="Z68" s="4" t="str">
@@ -6092,10 +6095,10 @@
         <v>0</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="4">
@@ -6147,7 +6150,7 @@
       <c r="W69" s="4"/>
       <c r="X69" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 63106, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 11737, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y69" s="4"/>
       <c r="Z69" s="4" t="str">
@@ -6160,10 +6163,10 @@
         <v>28</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="4">
@@ -6215,7 +6218,7 @@
       <c r="W70" s="4"/>
       <c r="X70" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 87013, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 73056, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y70" s="4"/>
       <c r="Z70" s="4" t="str">
@@ -6228,10 +6231,10 @@
         <v>57</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="4">
@@ -6283,7 +6286,7 @@
       <c r="W71" s="4"/>
       <c r="X71" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 42231, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 36570, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y71" s="4"/>
       <c r="Z71" s="4" t="str">
@@ -6296,10 +6299,10 @@
         <v>74</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="4">
@@ -6351,7 +6354,7 @@
       <c r="W72" s="4"/>
       <c r="X72" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 18658, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 25860, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y72" s="4"/>
       <c r="Z72" s="4" t="str">
@@ -6364,10 +6367,10 @@
         <v>24</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="4">
@@ -6419,7 +6422,7 @@
       <c r="W73" s="4"/>
       <c r="X73" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 45380, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 93101, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y73" s="4"/>
       <c r="Z73" s="4" t="str">
@@ -6432,10 +6435,10 @@
         <v>51</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="4">
@@ -6487,7 +6490,7 @@
       <c r="W74" s="4"/>
       <c r="X74" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 79254, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 56635, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y74" s="4"/>
       <c r="Z74" s="4" t="str">
@@ -6500,10 +6503,10 @@
         <v>3</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D75" s="8"/>
       <c r="E75" s="4">
@@ -6555,7 +6558,7 @@
       <c r="W75" s="4"/>
       <c r="X75" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 13568, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 66652, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y75" s="4"/>
       <c r="Z75" s="4" t="str">
@@ -6568,10 +6571,10 @@
         <v>14</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="4">
@@ -6623,7 +6626,7 @@
       <c r="W76" s="4"/>
       <c r="X76" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 35796, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 18891, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y76" s="4"/>
       <c r="Z76" s="4" t="str">
@@ -6636,10 +6639,10 @@
         <v>4</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="4">
@@ -6691,7 +6694,7 @@
       <c r="W77" s="4"/>
       <c r="X77" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 67258, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 53396, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y77" s="4"/>
       <c r="Z77" s="4" t="str">
@@ -6704,10 +6707,10 @@
         <v>16</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D78" s="8"/>
       <c r="E78" s="4">
@@ -6759,7 +6762,7 @@
       <c r="W78" s="4"/>
       <c r="X78" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 29725, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 92734, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y78" s="4"/>
       <c r="Z78" s="4" t="str">
@@ -6772,10 +6775,10 @@
         <v>32</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="4">
@@ -6827,7 +6830,7 @@
       <c r="W79" s="4"/>
       <c r="X79" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 53028, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 35632, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y79" s="4"/>
       <c r="Z79" s="4" t="str">
@@ -6840,10 +6843,10 @@
         <v>63</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="4">
@@ -6895,7 +6898,7 @@
       <c r="W80" s="4"/>
       <c r="X80" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 17574, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 97208, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y80" s="4"/>
       <c r="Z80" s="4" t="str">
@@ -6908,10 +6911,10 @@
         <v>49</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="4">
@@ -6963,7 +6966,7 @@
       <c r="W81" s="4"/>
       <c r="X81" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 59232, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 98007, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y81" s="4"/>
       <c r="Z81" s="4" t="str">
@@ -6976,10 +6979,10 @@
         <v>46</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="4">
@@ -7031,7 +7034,7 @@
       <c r="W82" s="4"/>
       <c r="X82" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 7773, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 868, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y82" s="4"/>
       <c r="Z82" s="4" t="str">
@@ -7044,10 +7047,10 @@
         <v>50</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="4">
@@ -7099,7 +7102,7 @@
       <c r="W83" s="4"/>
       <c r="X83" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 41704, 0 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 46995, 0 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4" t="str">
@@ -7112,10 +7115,10 @@
         <v>40</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="4">
@@ -7167,7 +7170,7 @@
       <c r="W84" s="4"/>
       <c r="X84" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 28907, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 11490, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y84" s="4"/>
       <c r="Z84" s="4" t="str">
@@ -7180,10 +7183,10 @@
         <v>39</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="4">
@@ -7235,7 +7238,7 @@
       <c r="W85" s="4"/>
       <c r="X85" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 19287, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 38118, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y85" s="4"/>
       <c r="Z85" s="4" t="str">
@@ -7248,10 +7251,10 @@
         <v>66</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="4">
@@ -7303,7 +7306,7 @@
       <c r="W86" s="4"/>
       <c r="X86" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 42745, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 14352, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y86" s="4"/>
       <c r="Z86" s="4" t="str">
@@ -7313,10 +7316,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="8"/>
@@ -7356,7 +7359,7 @@
         <v>Adrián</v>
       </c>
       <c r="R87" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S87" s="4"/>
       <c r="T87" s="5" t="s">
@@ -7370,7 +7373,7 @@
       <c r="W87" s="4"/>
       <c r="X87" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 38713, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 8581, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y87" s="4"/>
       <c r="Z87" s="4" t="str">
@@ -7380,10 +7383,10 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="8"/>
@@ -7423,7 +7426,7 @@
         <v>Agustín</v>
       </c>
       <c r="R88" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S88" s="4"/>
       <c r="T88" s="5" t="s">
@@ -7437,7 +7440,7 @@
       <c r="W88" s="4"/>
       <c r="X88" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 31269, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 21393, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y88" s="4"/>
       <c r="Z88" s="4" t="str">
@@ -7447,10 +7450,10 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="8"/>
@@ -7490,7 +7493,7 @@
         <v>Andrea</v>
       </c>
       <c r="R89" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S89" s="4"/>
       <c r="T89" s="5" t="s">
@@ -7504,7 +7507,7 @@
       <c r="W89" s="4"/>
       <c r="X89" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 66959, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 46033, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y89" s="4"/>
       <c r="Z89" s="4" t="str">
@@ -7514,10 +7517,10 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="8"/>
@@ -7557,7 +7560,7 @@
         <v>Ezequiel</v>
       </c>
       <c r="R90" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S90" s="4"/>
       <c r="T90" s="5" t="s">
@@ -7571,7 +7574,7 @@
       <c r="W90" s="4"/>
       <c r="X90" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 81117, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 8843, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y90" s="4"/>
       <c r="Z90" s="4" t="str">
@@ -7581,10 +7584,10 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>322</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>323</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="8"/>
@@ -7624,7 +7627,7 @@
         <v>Luis</v>
       </c>
       <c r="R91" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S91" s="4"/>
       <c r="T91" s="5" t="s">
@@ -7638,7 +7641,7 @@
       <c r="W91" s="4"/>
       <c r="X91" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 78257, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 5574, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y91" s="4"/>
       <c r="Z91" s="4" t="str">
@@ -7666,12 +7669,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0B7B36A0A09E458158046810038137" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bafe724513c9d1f26c4bf7dd6ed8389c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="03dca61d-4bd9-44e4-bb28-2e245975cefa" xmlns:ns4="58628ce2-31db-48c9-83e7-9ec9dce11b86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1eeb2709ac0754591c2d8728cadbcbe3" ns3:_="" ns4:_="">
     <xsd:import namespace="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
@@ -7880,6 +7877,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6844CB-EC2C-4324-A58D-DA98579E50A5}">
   <ds:schemaRefs>
@@ -7889,23 +7892,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2396B7-CB8B-47A8-AF89-5D1D70206F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7922,4 +7908,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minor changes for performance.
</commit_message>
<xml_diff>
--- a/database/Empleados.xlsx
+++ b/database/Empleados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\InnovationLab2019\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651DC3C6-A14D-419F-A485-38571747F6D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72172D01-7E2F-4A5A-BDA6-713809887069}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{77406EC5-31F3-4B7A-B386-A344DA39DCC7}"/>
   </bookViews>
@@ -1457,8 +1457,8 @@
   <dimension ref="A1:Z91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,7 +1586,7 @@
       <c r="W2" s="4"/>
       <c r="X2" s="4" t="str">
         <f ca="1">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q2, "', '", R2, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L2, " , ", IF(C2="", "NULL", CONCATENATE("'", B2,"/", C2, "'")),", ", K2, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B2,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 35784, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Belen', NULL, NULL, 76693, 0 , 'MVD/Adrian_Belen.JPG', 0 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4" t="str">
@@ -1654,7 +1654,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4" t="str">
         <f t="shared" ref="X3:X66" ca="1" si="13">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q3, "', '", R3, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L3, " , ", IF(C3="", "NULL", CONCATENATE("'", B3,"/", C3, "'")),", ", K3, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B3,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 6311, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Lopez', NULL, NULL, 65544, 0 , 'MVD/Adrian_Lopez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4" t="str">
@@ -1722,7 +1722,7 @@
       <c r="W4" s="4"/>
       <c r="X4" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 43714, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Da Cunha', NULL, NULL, 23064, 1 , 'MVD/Alberto_Dacunha.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4" t="str">
@@ -1788,7 +1788,7 @@
       <c r="W5" s="4"/>
       <c r="X5" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 20374, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alberto', 'Hernández', NULL, NULL, 88028, 0 , 'MVD/Alberto_Hernandez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4" t="str">
@@ -1856,7 +1856,7 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 84910, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Capece', NULL, NULL, 20356, 0 , 'MVD/Alejandro Capece.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4" t="str">
@@ -1924,7 +1924,7 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 26051, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alejandro', 'Latchinian', NULL, NULL, 63386, 0 , 'MVD/Alejandro_Latchinian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4" t="str">
@@ -1992,7 +1992,7 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 19037, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alfonso', 'Rodriguez', NULL, NULL, 63444, 1 , 'MVD/Alfonso_Rodriguez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4" t="str">
@@ -2060,7 +2060,7 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 52268, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Alvaro', 'Restuccia', NULL, NULL, 45464, 1 , 'MVD/Alvaro_Restuccia.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4" t="str">
@@ -2128,7 +2128,7 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 32425, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Bores', NULL, NULL, 81463, 0 , 'MVD/Andres_Bores.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4" t="str">
@@ -2196,7 +2196,7 @@
       <c r="W11" s="4"/>
       <c r="X11" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 45664, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Maedo', NULL, NULL, 39815, 1 , 'MVD/Andres_Maedo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4" t="str">
@@ -2264,7 +2264,7 @@
       <c r="W12" s="4"/>
       <c r="X12" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 92386, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrés', 'Nieves', NULL, NULL, 47509, 0 , 'MVD/Andres_Nieves.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4" t="str">
@@ -2332,7 +2332,7 @@
       <c r="W13" s="4"/>
       <c r="X13" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 7422, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Aniela', 'Amy', NULL, NULL, 58684, 0 , 'MVD/Aniela_Amy.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4" t="str">
@@ -2400,7 +2400,7 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 99959, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ariel', 'Sisro', NULL, NULL, 81250, 0 , 'MVD/Ariel_Sisro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4" t="str">
@@ -2468,7 +2468,7 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 15041, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Beerbal', 'Abdulkhader', NULL, NULL, 85069, 1 , 'MVD/Beerbal_Abdulkhader.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4" t="str">
@@ -2536,7 +2536,7 @@
       <c r="W16" s="4"/>
       <c r="X16" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 43661, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Bruno', 'Candia', NULL, NULL, 99229, 1 , 'MVD/Bruno_Candia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4" t="str">
@@ -2604,7 +2604,7 @@
       <c r="W17" s="4"/>
       <c r="X17" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 90404, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Roji', NULL, NULL, 21445, 0 , 'MVD/Camila_Roji.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4" t="str">
@@ -2672,7 +2672,7 @@
       <c r="W18" s="4"/>
       <c r="X18" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 98529, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camila', 'Sorio', NULL, NULL, 25508, 0 , 'MVD/Camila_Sorio.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4" t="str">
@@ -2740,7 +2740,7 @@
       <c r="W19" s="4"/>
       <c r="X19" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 88897, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Camilo', 'Gomez', NULL, NULL, 78605, 1 , 'MVD/Camilo_Gomez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4" t="str">
@@ -2808,7 +2808,7 @@
       <c r="W20" s="4"/>
       <c r="X20" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 29711, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Damián', 'Pereira', NULL, NULL, 12708, 1 , 'MVD/Damian_Pereira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4" t="str">
@@ -2876,7 +2876,7 @@
       <c r="W21" s="4"/>
       <c r="X21" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 68703, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Daniel', 'Cabrera', NULL, NULL, 23707, 0 , 'MVD/Daniel_Cabrera.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y21" s="4"/>
       <c r="Z21" s="4" t="str">
@@ -2944,7 +2944,7 @@
       <c r="W22" s="4"/>
       <c r="X22" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 14945, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Delia', 'Alvarez', NULL, NULL, 52674, 0 , 'MVD/Delia_Alvarez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y22" s="4"/>
       <c r="Z22" s="4" t="str">
@@ -3012,7 +3012,7 @@
       <c r="W23" s="4"/>
       <c r="X23" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 77885, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eduardo', 'Ducer', NULL, NULL, 86426, 0 , 'MVD/Eduardo_Ducer.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y23" s="4"/>
       <c r="Z23" s="4" t="str">
@@ -3080,7 +3080,7 @@
       <c r="W24" s="4"/>
       <c r="X24" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 30892, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Eugenia', 'Pais', NULL, NULL, 95498, 1 , 'MVD/Maria_Pais.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y24" s="4"/>
       <c r="Z24" s="4" t="str">
@@ -3148,7 +3148,7 @@
       <c r="W25" s="4"/>
       <c r="X25" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 49652, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Canet', NULL, NULL, 27469, 1 , 'MVD/Federico_Canet.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y25" s="4"/>
       <c r="Z25" s="4" t="str">
@@ -3216,7 +3216,7 @@
       <c r="W26" s="4"/>
       <c r="X26" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 28970, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'García', NULL, NULL, 73298, 0 , 'MVD/Federico_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y26" s="4"/>
       <c r="Z26" s="4" t="str">
@@ -3284,7 +3284,7 @@
       <c r="W27" s="4"/>
       <c r="X27" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 14927, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Federico', 'Trujillo', NULL, NULL, 35125, 1 , 'MVD/Federico_Trujillo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y27" s="4"/>
       <c r="Z27" s="4" t="str">
@@ -3352,7 +3352,7 @@
       <c r="W28" s="4"/>
       <c r="X28" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Olmos', NULL, NULL, 18091, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Olmos', NULL, NULL, 44046, 1 , 'MVD/Fernando_Olmos.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y28" s="4"/>
       <c r="Z28" s="4" t="str">
@@ -3420,7 +3420,7 @@
       <c r="W29" s="4"/>
       <c r="X29" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 14265, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Cañas', NULL, NULL, 10957, 0 , 'MVD/Fernando_Canas.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y29" s="4"/>
       <c r="Z29" s="4" t="str">
@@ -3488,7 +3488,7 @@
       <c r="W30" s="4"/>
       <c r="X30" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 99801, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Fernando', 'Stromillo', NULL, NULL, 95786, 0 , 'MVD/Fernando_Stromillo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y30" s="4"/>
       <c r="Z30" s="4" t="str">
@@ -3556,7 +3556,7 @@
       <c r="W31" s="4"/>
       <c r="X31" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 50773, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gastón', 'Aroztegui', NULL, NULL, 66755, 0 , 'MVD/Gaston_Aroztegui.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y31" s="4"/>
       <c r="Z31" s="4" t="str">
@@ -3624,7 +3624,7 @@
       <c r="W32" s="4"/>
       <c r="X32" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 39303, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Gerardo', 'Barbitta', NULL, NULL, 98952, 0 , 'MVD/Gerardo_Barbitta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y32" s="4"/>
       <c r="Z32" s="4" t="str">
@@ -3692,7 +3692,7 @@
       <c r="W33" s="4"/>
       <c r="X33" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 91940, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Giovanina', 'Chirione', NULL, NULL, 65840, 0 , 'MVD/Giovanina_Chirione.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y33" s="4"/>
       <c r="Z33" s="4" t="str">
@@ -3760,7 +3760,7 @@
       <c r="W34" s="4"/>
       <c r="X34" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 28288, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hernán', 'Rumbo', NULL, NULL, 48393, 0 , 'MVD/Hernan_Rumbo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y34" s="4"/>
       <c r="Z34" s="4" t="str">
@@ -3828,7 +3828,7 @@
       <c r="W35" s="4"/>
       <c r="X35" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 49637, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Horacio', 'Blanco', NULL, NULL, 78008, 0 , 'MVD/Horacio_Blanco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y35" s="4"/>
       <c r="Z35" s="4" t="str">
@@ -3896,7 +3896,7 @@
       <c r="W36" s="4"/>
       <c r="X36" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 7576, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Hugo', 'Ocampo', NULL, NULL, 65614, 0 , 'MVD/Hugo_Ocampo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y36" s="4"/>
       <c r="Z36" s="4" t="str">
@@ -3964,7 +3964,7 @@
       <c r="W37" s="4"/>
       <c r="X37" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 73354, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Assandri', NULL, NULL, 11239, 1 , 'MVD/Ignacio_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y37" s="4"/>
       <c r="Z37" s="4" t="str">
@@ -4032,7 +4032,7 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 5691, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Loureiro', NULL, NULL, 31377, 0 , 'MVD/Ignacio_Loureiro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y38" s="4"/>
       <c r="Z38" s="4" t="str">
@@ -4100,7 +4100,7 @@
       <c r="W39" s="4"/>
       <c r="X39" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 29540, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ignacio', 'Secco', NULL, NULL, 76639, 0 , 'MVD/Ignacio_Secco.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y39" s="4"/>
       <c r="Z39" s="4" t="str">
@@ -4168,7 +4168,7 @@
       <c r="W40" s="4"/>
       <c r="X40" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 74509, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Barrios', NULL, NULL, 72936, 0 , 'MVD/Javier_Barrios.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y40" s="4"/>
       <c r="Z40" s="4" t="str">
@@ -4236,7 +4236,7 @@
       <c r="W41" s="4"/>
       <c r="X41" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 3486, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Javier', 'Calero', NULL, NULL, 91840, 0 , 'MVD/Javier_Calero.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y41" s="4"/>
       <c r="Z41" s="4" t="str">
@@ -4304,7 +4304,7 @@
       <c r="W42" s="4"/>
       <c r="X42" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 39030, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jimena', 'Irigaray', NULL, NULL, 76175, 0 , 'MVD/Jimena_Irigaray.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y42" s="4"/>
       <c r="Z42" s="4" t="str">
@@ -4370,7 +4370,7 @@
       <c r="W43" s="4"/>
       <c r="X43" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 69887, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Jorge', 'Jova', NULL, NULL, 98737, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y43" s="4"/>
       <c r="Z43" s="4" t="str">
@@ -4438,7 +4438,7 @@
       <c r="W44" s="4"/>
       <c r="X44" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 77954, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Aguerre', NULL, NULL, 21690, 0 , 'MVD/Juan_Aguerre.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y44" s="4"/>
       <c r="Z44" s="4" t="str">
@@ -4506,7 +4506,7 @@
       <c r="W45" s="4"/>
       <c r="X45" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 37884, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan', 'Estrada', NULL, NULL, 95005, 0 , 'MVD/Juan_Estrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y45" s="4"/>
       <c r="Z45" s="4" t="str">
@@ -4574,7 +4574,7 @@
       <c r="W46" s="4"/>
       <c r="X46" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 40324, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Juan Manuel', 'Fagundez', NULL, NULL, 12224, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y46" s="4"/>
       <c r="Z46" s="4" t="str">
@@ -4646,7 +4646,7 @@
       <c r="W47" s="4"/>
       <c r="X47" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 60134, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Leonardo', 'Mendizabal', NULL, NULL, 73085, 0 , 'MVD/Leonardo_Mendizabal.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y47" s="4"/>
       <c r="Z47" s="4" t="str">
@@ -4714,7 +4714,7 @@
       <c r="W48" s="4"/>
       <c r="X48" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 39612, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luciano', 'Deluca', NULL, NULL, 78573, 0 , 'MVD/Luciano_Deluca.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y48" s="4"/>
       <c r="Z48" s="4" t="str">
@@ -4782,7 +4782,7 @@
       <c r="W49" s="4"/>
       <c r="X49" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 3929, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Malvina', 'Jaume', NULL, NULL, 77813, 0 , 'MVD/Malvina_Jaume.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y49" s="4"/>
       <c r="Z49" s="4" t="str">
@@ -4850,7 +4850,7 @@
       <c r="W50" s="4"/>
       <c r="X50" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 37694, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcelo', 'Zepedeo', NULL, NULL, 11910, 0 , 'MVD/Marcelo_Zepedeo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y50" s="4"/>
       <c r="Z50" s="4" t="str">
@@ -4918,7 +4918,7 @@
       <c r="W51" s="4"/>
       <c r="X51" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 29742, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marcos', 'Guimaraes', NULL, NULL, 59303, 0 , 'MVD/Marcos_Guimaraes.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y51" s="4"/>
       <c r="Z51" s="4" t="str">
@@ -4988,7 +4988,7 @@
       <c r="W52" s="4"/>
       <c r="X52" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 89047, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Julia', 'Etcheverry', NULL, NULL, 48489, 0 , 'MVD/Maria_Etcheverry.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y52" s="4"/>
       <c r="Z52" s="4" t="str">
@@ -5062,7 +5062,7 @@
       <c r="W53" s="4"/>
       <c r="X53" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 33754, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'María Noel', 'Mosqueira', NULL, NULL, 4762, 0 , 'MVD/Maria_Mosqueira.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y53" s="4"/>
       <c r="Z53" s="4" t="str">
@@ -5134,7 +5134,7 @@
       <c r="W54" s="4"/>
       <c r="X54" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 84184, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Marlon', 'González', NULL, NULL, 60863, 0 , 'MVD/Marlon_Gonzalez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y54" s="4"/>
       <c r="Z54" s="4" t="str">
@@ -5202,7 +5202,7 @@
       <c r="W55" s="4"/>
       <c r="X55" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 3588, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martín', 'Acosta', NULL, NULL, 73401, 0 , 'MVD/Martin_Acosta.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y55" s="4"/>
       <c r="Z55" s="4" t="str">
@@ -5270,7 +5270,7 @@
       <c r="W56" s="4"/>
       <c r="X56" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 13190, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Martin', 'Caetano', NULL, NULL, 88443, 0 , 'MVD/Martin_Caetano.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y56" s="4"/>
       <c r="Z56" s="4" t="str">
@@ -5338,7 +5338,7 @@
       <c r="W57" s="4"/>
       <c r="X57" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 14542, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mathías', 'Rodríguez', NULL, NULL, 80115, 1 , 'MVD/Mathias_Rodriguez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y57" s="4"/>
       <c r="Z57" s="4" t="str">
@@ -5406,7 +5406,7 @@
       <c r="W58" s="4"/>
       <c r="X58" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 59697, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Mauricio', 'Mora', NULL, NULL, 90379, 0 , 'MVD/Mauricio_Mora.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y58" s="4"/>
       <c r="Z58" s="4" t="str">
@@ -5474,7 +5474,7 @@
       <c r="W59" s="4"/>
       <c r="X59" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 40774, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Gómez', NULL, NULL, 21930, 1 , 'MVD/Nicolas_Gomez.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y59" s="4"/>
       <c r="Z59" s="4" t="str">
@@ -5542,7 +5542,7 @@
       <c r="W60" s="4"/>
       <c r="X60" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 5630, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolás', 'Lasarte', NULL, NULL, 93899, 1 , 'MVD/Nicolas_Lasarte.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y60" s="4"/>
       <c r="Z60" s="4" t="str">
@@ -5608,7 +5608,7 @@
       <c r="W61" s="4"/>
       <c r="X61" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 53862, 0 , 'MVD/Nicolas_Manay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Nicolas', 'Mañay', NULL, NULL, 37723, 0 , 'MVD/Nicolas_Manay.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y61" s="4"/>
       <c r="Z61" s="4" t="str">
@@ -5676,7 +5676,7 @@
       <c r="W62" s="4"/>
       <c r="X62" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 84708, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Octavio', 'Garbarino', NULL, NULL, 97600, 1 , 'MVD/Octavio_Garbarino.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y62" s="4"/>
       <c r="Z62" s="4" t="str">
@@ -5744,7 +5744,7 @@
       <c r="W63" s="4"/>
       <c r="X63" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 58230, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Cawen', NULL, NULL, 83267, 0 , 'MVD/Pablo_Cawen.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y63" s="4"/>
       <c r="Z63" s="4" t="str">
@@ -5812,7 +5812,7 @@
       <c r="W64" s="4"/>
       <c r="X64" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 97695, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Da Silva', NULL, NULL, 33893, 0 , 'MVD/Pablo_DaSilva.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y64" s="4"/>
       <c r="Z64" s="4" t="str">
@@ -5880,7 +5880,7 @@
       <c r="W65" s="4"/>
       <c r="X65" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 32040, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'García', NULL, NULL, 94150, 0 , 'MVD/Pablo_Garcia.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y65" s="4"/>
       <c r="Z65" s="4" t="str">
@@ -5946,7 +5946,7 @@
       <c r="W66" s="4"/>
       <c r="X66" s="4" t="str">
         <f t="shared" ca="1" si="13"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 29456, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Gus', NULL, NULL, 36962, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y66" s="4"/>
       <c r="Z66" s="4" t="str">
@@ -6014,7 +6014,7 @@
       <c r="W67" s="4"/>
       <c r="X67" s="4" t="str">
         <f t="shared" ref="X67:X91" ca="1" si="23">CONCATENATE("INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, '", Q67, "', '", R67, "', NULL, NULL, ", RANDBETWEEN(1, 100000), ", ", L67, " , ", IF(C67="", "NULL", CONCATENATE("'", B67,"/", C67, "'")),", ", K67, " FROM [dbo].[DeliveryUnit] WHERE [Code] = '", B67,"'")</f>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 46159, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Queirolo', NULL, NULL, 43140, 0 , 'MVD/Pablo_Queirolo.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y67" s="4"/>
       <c r="Z67" s="4" t="str">
@@ -6082,7 +6082,7 @@
       <c r="W68" s="4"/>
       <c r="X68" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 97358, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pablo', 'Uriarte', NULL, NULL, 53974, 0 , 'MVD/Pablo_Uriarte.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y68" s="4"/>
       <c r="Z68" s="4" t="str">
@@ -6150,7 +6150,7 @@
       <c r="W69" s="4"/>
       <c r="X69" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 11737, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Minetti', NULL, NULL, 13534, 0 , 'MVD/Pedro_Minetti.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y69" s="4"/>
       <c r="Z69" s="4" t="str">
@@ -6218,7 +6218,7 @@
       <c r="W70" s="4"/>
       <c r="X70" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 73056, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Pedro', 'Tournier', NULL, NULL, 42078, 1 , 'MVD/Pedro_Tournier.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y70" s="4"/>
       <c r="Z70" s="4" t="str">
@@ -6286,7 +6286,7 @@
       <c r="W71" s="4"/>
       <c r="X71" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 36570, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raidel', 'Gonzalez', NULL, NULL, 80495, 0 , 'MVD/Raidel_Gonzalez.jpeg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y71" s="4"/>
       <c r="Z71" s="4" t="str">
@@ -6354,7 +6354,7 @@
       <c r="W72" s="4"/>
       <c r="X72" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 25860, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Raúl', 'Fossemale', NULL, NULL, 88319, 0 , 'MVD/Raul_Fossemale.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y72" s="4"/>
       <c r="Z72" s="4" t="str">
@@ -6422,7 +6422,7 @@
       <c r="W73" s="4"/>
       <c r="X73" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 93101, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Roberto', 'Assandri', NULL, NULL, 34872, 0 , 'MVD/Roberto_Assandri.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y73" s="4"/>
       <c r="Z73" s="4" t="str">
@@ -6490,7 +6490,7 @@
       <c r="W74" s="4"/>
       <c r="X74" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 56635, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Alvarez', NULL, NULL, 16699, 0 , 'MVD/Rodrigo_Alvarez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y74" s="4"/>
       <c r="Z74" s="4" t="str">
@@ -6558,7 +6558,7 @@
       <c r="W75" s="4"/>
       <c r="X75" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 66652, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Rodrigo', 'Valdez', NULL, NULL, 3347, 0 , 'MVD/Rodrigo_Valdez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y75" s="4"/>
       <c r="Z75" s="4" t="str">
@@ -6626,7 +6626,7 @@
       <c r="W76" s="4"/>
       <c r="X76" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 18891, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ruben', 'Bracco', NULL, NULL, 94, 0 , 'MVD/Ruben_Bracco.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y76" s="4"/>
       <c r="Z76" s="4" t="str">
@@ -6694,7 +6694,7 @@
       <c r="W77" s="4"/>
       <c r="X77" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 53396, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Santiago', 'Ferreiro', NULL, NULL, 96249, 0 , 'MVD/Santiago_Ferreiro.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y77" s="4"/>
       <c r="Z77" s="4" t="str">
@@ -6762,7 +6762,7 @@
       <c r="W78" s="4"/>
       <c r="X78" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 92734, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Sebastian', 'Queirolo', NULL, NULL, 65062, 0 , 'MVD/Sebastian_Queirolo.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y78" s="4"/>
       <c r="Z78" s="4" t="str">
@@ -6830,7 +6830,7 @@
       <c r="W79" s="4"/>
       <c r="X79" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 35632, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Silvia', 'Derkoyorikian', NULL, NULL, 19046, 0 , 'MVD/Silvia_Derkoyorikian.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y79" s="4"/>
       <c r="Z79" s="4" t="str">
@@ -6898,7 +6898,7 @@
       <c r="W80" s="4"/>
       <c r="X80" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 97208, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valentín', 'Gadola', NULL, NULL, 76051, 0 , 'MVD/Valentin_Gadola.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y80" s="4"/>
       <c r="Z80" s="4" t="str">
@@ -6966,7 +6966,7 @@
       <c r="W81" s="4"/>
       <c r="X81" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 98007, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Valeria', 'Rotunno', NULL, NULL, 25620, 0 , 'MVD/Valeria_Rotunno.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y81" s="4"/>
       <c r="Z81" s="4" t="str">
@@ -7034,7 +7034,7 @@
       <c r="W82" s="4"/>
       <c r="X82" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 868, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Victoria', 'Andrada', NULL, NULL, 39321, 0 , 'MVD/Victoria_Andrada.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y82" s="4"/>
       <c r="Z82" s="4" t="str">
@@ -7072,7 +7072,7 @@
         <v>1</v>
       </c>
       <c r="L83" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" s="4" t="str">
@@ -7102,7 +7102,7 @@
       <c r="W83" s="4"/>
       <c r="X83" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 46995, 0 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'William', 'Claro', NULL, NULL, 8917, 1 , 'MVD/William_Claro.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y83" s="4"/>
       <c r="Z83" s="4" t="str">
@@ -7170,7 +7170,7 @@
       <c r="W84" s="4"/>
       <c r="X84" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 11490, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yago', 'Auza', NULL, NULL, 48062, 0 , 'MVD/Yago_Auza.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y84" s="4"/>
       <c r="Z84" s="4" t="str">
@@ -7238,7 +7238,7 @@
       <c r="W85" s="4"/>
       <c r="X85" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 38118, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yanara', 'Valdes', NULL, NULL, 75444, 0 , 'MVD/Yanara_Valdes.jpg', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y85" s="4"/>
       <c r="Z85" s="4" t="str">
@@ -7306,7 +7306,7 @@
       <c r="W86" s="4"/>
       <c r="X86" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 14352, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Yony', 'Gómez', NULL, NULL, 83704, 0 , 'MVD/Yony_Gomez.JPG', 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'MVD'</v>
       </c>
       <c r="Y86" s="4"/>
       <c r="Z86" s="4" t="str">
@@ -7373,7 +7373,7 @@
       <c r="W87" s="4"/>
       <c r="X87" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 8581, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Adrián', 'Costa', NULL, NULL, 49726, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y87" s="4"/>
       <c r="Z87" s="4" t="str">
@@ -7440,7 +7440,7 @@
       <c r="W88" s="4"/>
       <c r="X88" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 21393, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Agustín', 'Narvaez', NULL, NULL, 50347, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y88" s="4"/>
       <c r="Z88" s="4" t="str">
@@ -7507,7 +7507,7 @@
       <c r="W89" s="4"/>
       <c r="X89" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 46033, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Andrea', 'Sabella', NULL, NULL, 24736, 1 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y89" s="4"/>
       <c r="Z89" s="4" t="str">
@@ -7574,7 +7574,7 @@
       <c r="W90" s="4"/>
       <c r="X90" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 8843, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Ezequiel', 'Konjuh', NULL, NULL, 19458, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y90" s="4"/>
       <c r="Z90" s="4" t="str">
@@ -7641,7 +7641,7 @@
       <c r="W91" s="4"/>
       <c r="X91" s="4" t="str">
         <f t="shared" ca="1" si="23"/>
-        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 5574, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
+        <v>INSERT INTO [dbo].[Candidate] ([DeliveryUnitId], [RelationType], [FirstName], [LastName], [DocType], [DocNumber], [EmployeeNumber], [InBench], [Picture], [IsActive]) SELECT [Id], 1, 'Luis', 'Fregeiro', NULL, NULL, 603, 0 , NULL, 1 FROM [dbo].[DeliveryUnit] WHERE [Code] = 'ROS'</v>
       </c>
       <c r="Y91" s="4"/>
       <c r="Z91" s="4" t="str">
@@ -7669,6 +7669,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0B7B36A0A09E458158046810038137" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bafe724513c9d1f26c4bf7dd6ed8389c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="03dca61d-4bd9-44e4-bb28-2e245975cefa" xmlns:ns4="58628ce2-31db-48c9-83e7-9ec9dce11b86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1eeb2709ac0754591c2d8728cadbcbe3" ns3:_="" ns4:_="">
     <xsd:import namespace="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
@@ -7877,12 +7883,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6844CB-EC2C-4324-A58D-DA98579E50A5}">
   <ds:schemaRefs>
@@ -7892,6 +7892,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2396B7-CB8B-47A8-AF89-5D1D70206F99}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7908,21 +7925,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2B1C0-C05E-43DF-9662-E26ED0AB0738}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="58628ce2-31db-48c9-83e7-9ec9dce11b86"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="03dca61d-4bd9-44e4-bb28-2e245975cefa"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>